<commit_message>
removed a few bugs, cleaned up some visulizations
</commit_message>
<xml_diff>
--- a/development/centroids_excel.xlsx
+++ b/development/centroids_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexalmond/IAS-150/development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0225C4D2-0A5C-BA45-80A5-D711F454D1A1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB99ADD-7ED7-C94E-971C-4908A5F61EB6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{AC191E4E-968C-6248-B7AF-0668A78F736C}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <t>CI</t>
   </si>
   <si>
-    <t>Côte d'Ivoire</t>
-  </si>
-  <si>
     <t>CK</t>
   </si>
   <si>
@@ -1510,6 +1507,9 @@
   </si>
   <si>
     <t>State of Palestine</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
   </si>
 </sst>
 </file>
@@ -1870,24 +1870,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BFDB36-F6CC-5441-B7FD-44B27C79474A}">
   <dimension ref="A1:D248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -2475,12 +2475,12 @@
         <v>-5.5470800000000002</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>82</v>
+        <v>494</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="1">
         <v>-21.236736000000001</v>
@@ -2489,12 +2489,12 @@
         <v>-159.777671</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B45" s="1">
         <v>-35.675147000000003</v>
@@ -2503,12 +2503,12 @@
         <v>-71.542968999999999</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" s="1">
         <v>7.3697220000000003</v>
@@ -2517,12 +2517,12 @@
         <v>12.354722000000001</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B47" s="1">
         <v>35.861660000000001</v>
@@ -2531,12 +2531,12 @@
         <v>104.195397</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1">
         <v>4.5708679999999999</v>
@@ -2545,12 +2545,12 @@
         <v>-74.297332999999995</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="1">
         <v>9.7489170000000005</v>
@@ -2559,12 +2559,12 @@
         <v>-83.753428</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" s="1">
         <v>21.521757000000001</v>
@@ -2573,12 +2573,12 @@
         <v>-77.781166999999996</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" s="1">
         <v>16.002082000000001</v>
@@ -2587,12 +2587,12 @@
         <v>-24.013197000000002</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="1">
         <v>-10.447525000000001</v>
@@ -2601,12 +2601,12 @@
         <v>105.690449</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" s="1">
         <v>35.126412999999999</v>
@@ -2615,12 +2615,12 @@
         <v>33.429859</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="1">
         <v>49.817492000000001</v>
@@ -2629,12 +2629,12 @@
         <v>15.472962000000001</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B55" s="1">
         <v>51.165691000000002</v>
@@ -2643,12 +2643,12 @@
         <v>10.451525999999999</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B56" s="1">
         <v>11.825138000000001</v>
@@ -2657,12 +2657,12 @@
         <v>42.590274999999998</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B57" s="1">
         <v>56.263919999999999</v>
@@ -2671,12 +2671,12 @@
         <v>9.5017849999999999</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B58" s="1">
         <v>15.414999</v>
@@ -2685,12 +2685,12 @@
         <v>-61.370975999999999</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B59" s="1">
         <v>18.735693000000001</v>
@@ -2699,12 +2699,12 @@
         <v>-70.162650999999997</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B60" s="1">
         <v>28.033885999999999</v>
@@ -2713,12 +2713,12 @@
         <v>1.659626</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="1">
         <v>-1.8312390000000001</v>
@@ -2727,12 +2727,12 @@
         <v>-78.183406000000005</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B62" s="1">
         <v>58.595272000000001</v>
@@ -2741,12 +2741,12 @@
         <v>25.013607</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B63" s="1">
         <v>26.820553</v>
@@ -2755,12 +2755,12 @@
         <v>30.802498</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B64" s="1">
         <v>24.215527000000002</v>
@@ -2769,12 +2769,12 @@
         <v>-12.885833999999999</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B65" s="1">
         <v>15.179384000000001</v>
@@ -2783,12 +2783,12 @@
         <v>39.782333999999999</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B66" s="1">
         <v>40.463667000000001</v>
@@ -2797,12 +2797,12 @@
         <v>-3.7492200000000002</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1">
         <v>9.1449999999999996</v>
@@ -2811,12 +2811,12 @@
         <v>40.489673000000003</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B68" s="1">
         <v>61.924109999999999</v>
@@ -2825,12 +2825,12 @@
         <v>25.748151</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B69" s="1">
         <v>-16.578192999999999</v>
@@ -2839,12 +2839,12 @@
         <v>179.414413</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B70" s="1">
         <v>-51.796253</v>
@@ -2853,12 +2853,12 @@
         <v>-59.523612999999997</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B71" s="1">
         <v>7.425554</v>
@@ -2867,12 +2867,12 @@
         <v>150.55081200000001</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B72" s="1">
         <v>61.892634999999999</v>
@@ -2881,12 +2881,12 @@
         <v>-6.9118060000000003</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B73" s="1">
         <v>46.227637999999999</v>
@@ -2895,12 +2895,12 @@
         <v>2.213749</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B74" s="1">
         <v>-0.80368899999999999</v>
@@ -2909,12 +2909,12 @@
         <v>11.609444</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B75" s="1">
         <v>55.378050999999999</v>
@@ -2923,12 +2923,12 @@
         <v>-3.4359730000000002</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B76" s="1">
         <v>12.262776000000001</v>
@@ -2937,12 +2937,12 @@
         <v>-61.604171000000001</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B77" s="1">
         <v>42.315407</v>
@@ -2951,12 +2951,12 @@
         <v>43.356892000000002</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B78" s="1">
         <v>3.9338890000000002</v>
@@ -2965,12 +2965,12 @@
         <v>-53.125782000000001</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B79" s="1">
         <v>49.465691</v>
@@ -2979,12 +2979,12 @@
         <v>-2.5852780000000002</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B80" s="1">
         <v>7.9465269999999997</v>
@@ -2993,12 +2993,12 @@
         <v>-1.0231939999999999</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B81" s="1">
         <v>36.137740999999998</v>
@@ -3007,12 +3007,12 @@
         <v>-5.3453739999999996</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B82" s="1">
         <v>71.706935999999999</v>
@@ -3021,12 +3021,12 @@
         <v>-42.604303000000002</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B83" s="1">
         <v>13.443182</v>
@@ -3035,12 +3035,12 @@
         <v>-15.310138999999999</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B84" s="1">
         <v>9.9455869999999997</v>
@@ -3049,12 +3049,12 @@
         <v>-9.6966450000000002</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B85" s="1">
         <v>16.995971000000001</v>
@@ -3063,12 +3063,12 @@
         <v>-62.067641000000002</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B86" s="1">
         <v>1.650801</v>
@@ -3077,12 +3077,12 @@
         <v>10.267894999999999</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B87" s="1">
         <v>39.074207999999999</v>
@@ -3091,12 +3091,12 @@
         <v>21.824311999999999</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B88" s="1">
         <v>-54.429578999999997</v>
@@ -3105,12 +3105,12 @@
         <v>-36.587909000000003</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B89" s="1">
         <v>15.783471</v>
@@ -3119,12 +3119,12 @@
         <v>-90.230759000000006</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B90" s="1">
         <v>13.444304000000001</v>
@@ -3133,12 +3133,12 @@
         <v>144.79373100000001</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B91" s="1">
         <v>11.803749</v>
@@ -3147,12 +3147,12 @@
         <v>-15.180413</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B92" s="1">
         <v>4.8604159999999998</v>
@@ -3161,12 +3161,12 @@
         <v>-58.93018</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B93" s="1">
         <v>31.354676000000001</v>
@@ -3175,12 +3175,12 @@
         <v>34.308824999999999</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B94" s="1">
         <v>22.396428</v>
@@ -3189,12 +3189,12 @@
         <v>114.109497</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B95" s="1">
         <v>-53.081809999999997</v>
@@ -3203,12 +3203,12 @@
         <v>73.504158000000004</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B96" s="1">
         <v>15.199999</v>
@@ -3217,12 +3217,12 @@
         <v>-86.241905000000003</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B97" s="1">
         <v>45.1</v>
@@ -3231,12 +3231,12 @@
         <v>15.2</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B98" s="1">
         <v>18.971187</v>
@@ -3245,12 +3245,12 @@
         <v>-72.285214999999994</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B99" s="1">
         <v>47.162494000000002</v>
@@ -3259,12 +3259,12 @@
         <v>19.503304</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B100" s="1">
         <v>-0.78927499999999995</v>
@@ -3273,12 +3273,12 @@
         <v>113.92132700000001</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B101" s="1">
         <v>53.412909999999997</v>
@@ -3287,12 +3287,12 @@
         <v>-8.2438900000000004</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B102" s="1">
         <v>31.046050999999999</v>
@@ -3301,12 +3301,12 @@
         <v>34.851612000000003</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B103" s="1">
         <v>54.236106999999997</v>
@@ -3315,12 +3315,12 @@
         <v>-4.5480559999999999</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B104" s="1">
         <v>20.593684</v>
@@ -3329,12 +3329,12 @@
         <v>78.962879999999998</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B105" s="1">
         <v>-6.3431940000000004</v>
@@ -3343,12 +3343,12 @@
         <v>71.876519000000002</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B106" s="1">
         <v>33.223191</v>
@@ -3357,12 +3357,12 @@
         <v>43.679290999999999</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B107" s="1">
         <v>32.427908000000002</v>
@@ -3371,12 +3371,12 @@
         <v>53.688046</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B108" s="1">
         <v>64.963050999999993</v>
@@ -3385,12 +3385,12 @@
         <v>-19.020835000000002</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B109" s="1">
         <v>41.871940000000002</v>
@@ -3399,12 +3399,12 @@
         <v>12.56738</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B110" s="1">
         <v>49.214438999999999</v>
@@ -3413,12 +3413,12 @@
         <v>-2.1312500000000001</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B111" s="1">
         <v>18.109580999999999</v>
@@ -3427,12 +3427,12 @@
         <v>-77.297507999999993</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B112" s="1">
         <v>30.585163999999999</v>
@@ -3441,12 +3441,12 @@
         <v>36.238413999999999</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B113" s="1">
         <v>36.204824000000002</v>
@@ -3455,12 +3455,12 @@
         <v>138.25292400000001</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B114" s="1">
         <v>-2.3559E-2</v>
@@ -3469,12 +3469,12 @@
         <v>37.906193000000002</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B115" s="1">
         <v>41.20438</v>
@@ -3483,12 +3483,12 @@
         <v>74.766098</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B116" s="1">
         <v>12.565678999999999</v>
@@ -3497,12 +3497,12 @@
         <v>104.99096299999999</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B117" s="1">
         <v>-3.3704170000000002</v>
@@ -3511,12 +3511,12 @@
         <v>-168.734039</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B118" s="1">
         <v>-11.875000999999999</v>
@@ -3525,12 +3525,12 @@
         <v>43.872219000000001</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B119" s="1">
         <v>17.357821999999999</v>
@@ -3539,12 +3539,12 @@
         <v>-62.782997999999999</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B120" s="1">
         <v>40.339852</v>
@@ -3553,12 +3553,12 @@
         <v>127.510093</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B121" s="1">
         <v>35.907756999999997</v>
@@ -3567,12 +3567,12 @@
         <v>127.76692199999999</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B122" s="1">
         <v>29.31166</v>
@@ -3581,12 +3581,12 @@
         <v>47.481766</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B123" s="1">
         <v>19.513469000000001</v>
@@ -3595,12 +3595,12 @@
         <v>-80.566956000000005</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B124" s="1">
         <v>48.019573000000001</v>
@@ -3609,12 +3609,12 @@
         <v>66.923683999999994</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B125" s="1">
         <v>19.856269999999999</v>
@@ -3623,12 +3623,12 @@
         <v>102.495496</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B126" s="1">
         <v>33.854720999999998</v>
@@ -3637,12 +3637,12 @@
         <v>35.862285</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B127" s="1">
         <v>13.909444000000001</v>
@@ -3651,12 +3651,12 @@
         <v>-60.978892999999999</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B128" s="1">
         <v>47.165999999999997</v>
@@ -3665,12 +3665,12 @@
         <v>9.5553729999999995</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B129" s="1">
         <v>7.8730539999999998</v>
@@ -3679,12 +3679,12 @@
         <v>80.771797000000007</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B130" s="1">
         <v>6.4280549999999996</v>
@@ -3693,12 +3693,12 @@
         <v>-9.4294989999999999</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B131" s="1">
         <v>-29.609988000000001</v>
@@ -3707,12 +3707,12 @@
         <v>28.233608</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B132" s="1">
         <v>55.169438</v>
@@ -3721,12 +3721,12 @@
         <v>23.881274999999999</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B133" s="1">
         <v>49.815272999999998</v>
@@ -3735,12 +3735,12 @@
         <v>6.1295830000000002</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B134" s="1">
         <v>56.879635</v>
@@ -3749,12 +3749,12 @@
         <v>24.603189</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B135" s="1">
         <v>26.335100000000001</v>
@@ -3763,12 +3763,12 @@
         <v>17.228331000000001</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B136" s="1">
         <v>31.791702000000001</v>
@@ -3777,12 +3777,12 @@
         <v>-7.0926200000000001</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B137" s="1">
         <v>43.750298000000001</v>
@@ -3791,12 +3791,12 @@
         <v>7.4128410000000002</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B138" s="1">
         <v>47.411631</v>
@@ -3805,12 +3805,12 @@
         <v>28.369885</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B139" s="1">
         <v>42.708677999999999</v>
@@ -3819,12 +3819,12 @@
         <v>19.374389999999998</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B140" s="1">
         <v>-18.766946999999998</v>
@@ -3833,12 +3833,12 @@
         <v>46.869107</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B141" s="1">
         <v>7.1314739999999999</v>
@@ -3847,12 +3847,12 @@
         <v>171.18447800000001</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B142" s="1">
         <v>41.608635</v>
@@ -3861,12 +3861,12 @@
         <v>21.745274999999999</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B143" s="1">
         <v>17.570692000000001</v>
@@ -3875,12 +3875,12 @@
         <v>-3.9961660000000001</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B144" s="1">
         <v>21.913965000000001</v>
@@ -3889,12 +3889,12 @@
         <v>95.956222999999994</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B145" s="1">
         <v>46.862496</v>
@@ -3903,12 +3903,12 @@
         <v>103.846656</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B146" s="1">
         <v>22.198744999999999</v>
@@ -3917,12 +3917,12 @@
         <v>113.543873</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B147" s="1">
         <v>17.330829999999999</v>
@@ -3931,12 +3931,12 @@
         <v>145.38469000000001</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B148" s="1">
         <v>14.641527999999999</v>
@@ -3945,12 +3945,12 @@
         <v>-61.024174000000002</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B149" s="1">
         <v>21.00789</v>
@@ -3959,12 +3959,12 @@
         <v>-10.940835</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B150" s="1">
         <v>16.742498000000001</v>
@@ -3973,12 +3973,12 @@
         <v>-62.187365999999997</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B151" s="1">
         <v>35.937496000000003</v>
@@ -3987,12 +3987,12 @@
         <v>14.375416</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B152" s="1">
         <v>-20.348403999999999</v>
@@ -4001,12 +4001,12 @@
         <v>57.552152</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B153" s="1">
         <v>3.2027779999999999</v>
@@ -4015,12 +4015,12 @@
         <v>73.220680000000002</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B154" s="1">
         <v>-13.254308</v>
@@ -4029,12 +4029,12 @@
         <v>34.301524999999998</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B155" s="1">
         <v>23.634501</v>
@@ -4043,12 +4043,12 @@
         <v>-102.552784</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B156" s="1">
         <v>4.2104840000000001</v>
@@ -4057,12 +4057,12 @@
         <v>101.97576599999999</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B157" s="1">
         <v>-18.665694999999999</v>
@@ -4071,12 +4071,12 @@
         <v>35.529561999999999</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B158" s="1">
         <v>-22.957640000000001</v>
@@ -4085,12 +4085,12 @@
         <v>18.490410000000001</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B159" s="1">
         <v>-20.904305000000001</v>
@@ -4099,12 +4099,12 @@
         <v>165.618042</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B160" s="1">
         <v>17.607789</v>
@@ -4113,12 +4113,12 @@
         <v>8.0816660000000002</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B161" s="1">
         <v>-29.040835000000001</v>
@@ -4127,12 +4127,12 @@
         <v>167.954712</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B162" s="1">
         <v>9.0819989999999997</v>
@@ -4141,12 +4141,12 @@
         <v>8.6752769999999995</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B163" s="1">
         <v>12.865416</v>
@@ -4155,12 +4155,12 @@
         <v>-85.207228999999998</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B164" s="1">
         <v>52.132632999999998</v>
@@ -4169,12 +4169,12 @@
         <v>5.2912660000000002</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B165" s="1">
         <v>60.472023999999998</v>
@@ -4183,12 +4183,12 @@
         <v>8.4689460000000008</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B166" s="1">
         <v>28.394856999999998</v>
@@ -4197,12 +4197,12 @@
         <v>84.124008000000003</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B167" s="1">
         <v>-0.52277799999999996</v>
@@ -4211,12 +4211,12 @@
         <v>166.93150299999999</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B168" s="1">
         <v>-19.054445000000001</v>
@@ -4225,12 +4225,12 @@
         <v>-169.867233</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B169" s="1">
         <v>-40.900556999999999</v>
@@ -4239,12 +4239,12 @@
         <v>174.88597100000001</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B170" s="1">
         <v>21.512582999999999</v>
@@ -4253,12 +4253,12 @@
         <v>55.923254999999997</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B171" s="1">
         <v>8.5379810000000003</v>
@@ -4267,12 +4267,12 @@
         <v>-80.782127000000003</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B172" s="1">
         <v>-9.1899669999999993</v>
@@ -4281,12 +4281,12 @@
         <v>-75.015152</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B173" s="1">
         <v>-17.679742000000001</v>
@@ -4295,12 +4295,12 @@
         <v>-149.40684300000001</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B174" s="1">
         <v>-6.3149930000000003</v>
@@ -4309,12 +4309,12 @@
         <v>143.95554999999999</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B175" s="1">
         <v>12.879721</v>
@@ -4323,12 +4323,12 @@
         <v>121.774017</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B176" s="1">
         <v>30.375321</v>
@@ -4337,12 +4337,12 @@
         <v>69.345116000000004</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B177" s="1">
         <v>51.919438</v>
@@ -4351,12 +4351,12 @@
         <v>19.145136000000001</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B178" s="1">
         <v>46.941935999999998</v>
@@ -4365,12 +4365,12 @@
         <v>-56.27111</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B179" s="1">
         <v>-24.703614999999999</v>
@@ -4379,12 +4379,12 @@
         <v>-127.439308</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B180" s="1">
         <v>18.220832999999999</v>
@@ -4393,12 +4393,12 @@
         <v>-66.590148999999997</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B181" s="1">
         <v>31.952162000000001</v>
@@ -4407,12 +4407,12 @@
         <v>35.233153999999999</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B182" s="1">
         <v>39.399872000000002</v>
@@ -4421,12 +4421,12 @@
         <v>-8.2244539999999997</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B183" s="1">
         <v>7.5149800000000004</v>
@@ -4435,12 +4435,12 @@
         <v>134.58251999999999</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B184" s="1">
         <v>-23.442502999999999</v>
@@ -4449,12 +4449,12 @@
         <v>-58.443832</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B185" s="1">
         <v>25.354825999999999</v>
@@ -4463,12 +4463,12 @@
         <v>51.183883999999999</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B186" s="1">
         <v>-21.115141000000001</v>
@@ -4477,12 +4477,12 @@
         <v>55.536383999999998</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B187" s="1">
         <v>45.943161000000003</v>
@@ -4491,12 +4491,12 @@
         <v>24.966760000000001</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B188" s="1">
         <v>44.016520999999997</v>
@@ -4505,12 +4505,12 @@
         <v>21.005859000000001</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B189" s="1">
         <v>61.524009999999997</v>
@@ -4519,12 +4519,12 @@
         <v>105.31875599999999</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B190" s="1">
         <v>-1.9402779999999999</v>
@@ -4533,12 +4533,12 @@
         <v>29.873888000000001</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B191" s="1">
         <v>23.885942</v>
@@ -4547,12 +4547,12 @@
         <v>45.079161999999997</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B192" s="1">
         <v>-9.6457099999999993</v>
@@ -4561,12 +4561,12 @@
         <v>160.156194</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B193" s="1">
         <v>-4.6795739999999997</v>
@@ -4575,12 +4575,12 @@
         <v>55.491976999999999</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B194" s="1">
         <v>12.862807</v>
@@ -4589,12 +4589,12 @@
         <v>30.217635999999999</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B195" s="1">
         <v>60.128160999999999</v>
@@ -4603,12 +4603,12 @@
         <v>18.643501000000001</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B196" s="1">
         <v>1.3520829999999999</v>
@@ -4617,12 +4617,12 @@
         <v>103.819836</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B197" s="1">
         <v>-24.143474000000001</v>
@@ -4631,12 +4631,12 @@
         <v>-10.030696000000001</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B198" s="1">
         <v>46.151240999999999</v>
@@ -4645,12 +4645,12 @@
         <v>14.995463000000001</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B199" s="1">
         <v>77.553604000000007</v>
@@ -4659,12 +4659,12 @@
         <v>23.670272000000001</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B200" s="1">
         <v>48.669026000000002</v>
@@ -4673,12 +4673,12 @@
         <v>19.699024000000001</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B201" s="1">
         <v>8.4605549999999994</v>
@@ -4687,12 +4687,12 @@
         <v>-11.779889000000001</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B202" s="1">
         <v>43.942360000000001</v>
@@ -4701,12 +4701,12 @@
         <v>12.457777</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B203" s="1">
         <v>14.497401</v>
@@ -4715,12 +4715,12 @@
         <v>-14.452362000000001</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B204" s="1">
         <v>5.1521489999999996</v>
@@ -4729,12 +4729,12 @@
         <v>46.199615999999999</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B205" s="1">
         <v>3.919305</v>
@@ -4743,12 +4743,12 @@
         <v>-56.027782999999999</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B206" s="1">
         <v>0.18636</v>
@@ -4757,12 +4757,12 @@
         <v>6.6130810000000002</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B207" s="1">
         <v>13.794185000000001</v>
@@ -4771,12 +4771,12 @@
         <v>-88.896529999999998</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B208" s="1">
         <v>34.802075000000002</v>
@@ -4785,12 +4785,12 @@
         <v>38.996814999999998</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B209" s="1">
         <v>-26.522503</v>
@@ -4799,12 +4799,12 @@
         <v>31.465865999999998</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B210" s="1">
         <v>21.694025</v>
@@ -4813,12 +4813,12 @@
         <v>-71.797927999999999</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B211" s="1">
         <v>15.454166000000001</v>
@@ -4827,12 +4827,12 @@
         <v>18.732206999999999</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B212" s="1">
         <v>-49.280366000000001</v>
@@ -4841,12 +4841,12 @@
         <v>69.348557</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B213" s="1">
         <v>8.6195430000000002</v>
@@ -4855,12 +4855,12 @@
         <v>0.82478200000000002</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B214" s="1">
         <v>15.870032</v>
@@ -4869,12 +4869,12 @@
         <v>100.992541</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B215" s="1">
         <v>38.861033999999997</v>
@@ -4883,12 +4883,12 @@
         <v>71.276093000000003</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B216" s="1">
         <v>-8.9673630000000006</v>
@@ -4897,12 +4897,12 @@
         <v>-171.85588100000001</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B217" s="1">
         <v>-8.8742169999999998</v>
@@ -4911,12 +4911,12 @@
         <v>125.72753899999999</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B218" s="1">
         <v>38.969718999999998</v>
@@ -4925,12 +4925,12 @@
         <v>59.556277999999999</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B219" s="1">
         <v>33.886916999999997</v>
@@ -4939,12 +4939,12 @@
         <v>9.5374990000000004</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B220" s="1">
         <v>-21.178985999999998</v>
@@ -4953,12 +4953,12 @@
         <v>-175.19824199999999</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B221" s="1">
         <v>38.963745000000003</v>
@@ -4967,12 +4967,12 @@
         <v>35.243321999999999</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B222" s="1">
         <v>10.691803</v>
@@ -4981,12 +4981,12 @@
         <v>-61.222503000000003</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B223" s="1">
         <v>-7.1095350000000002</v>
@@ -4995,12 +4995,12 @@
         <v>177.64932999999999</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B224" s="1">
         <v>23.69781</v>
@@ -5009,12 +5009,12 @@
         <v>120.960515</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B225" s="1">
         <v>-6.3690280000000001</v>
@@ -5023,12 +5023,12 @@
         <v>34.888821999999998</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B226" s="1">
         <v>48.379432999999999</v>
@@ -5037,12 +5037,12 @@
         <v>31.165579999999999</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B227" s="1">
         <v>1.3733329999999999</v>
@@ -5051,12 +5051,12 @@
         <v>32.290275000000001</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B228" s="1">
         <v>0</v>
@@ -5065,12 +5065,12 @@
         <v>0</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B229" s="1">
         <v>37.090240000000001</v>
@@ -5079,12 +5079,12 @@
         <v>-95.712890999999999</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B230" s="1">
         <v>-32.522779</v>
@@ -5093,12 +5093,12 @@
         <v>-55.765835000000003</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B231" s="1">
         <v>41.377490999999999</v>
@@ -5107,12 +5107,12 @@
         <v>64.585262</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B232" s="1">
         <v>41.902915999999998</v>
@@ -5121,12 +5121,12 @@
         <v>12.453389</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B233" s="1">
         <v>12.984305000000001</v>
@@ -5135,12 +5135,12 @@
         <v>-61.287227999999999</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="234" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B234" s="1">
         <v>6.4237500000000001</v>
@@ -5149,12 +5149,12 @@
         <v>-66.589730000000003</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B235" s="1">
         <v>18.420694999999998</v>
@@ -5163,12 +5163,12 @@
         <v>-64.639967999999996</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B236" s="1">
         <v>18.335764999999999</v>
@@ -5177,12 +5177,12 @@
         <v>-64.896334999999993</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B237" s="1">
         <v>14.058324000000001</v>
@@ -5191,12 +5191,12 @@
         <v>108.277199</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B238" s="1">
         <v>-15.376706</v>
@@ -5205,12 +5205,12 @@
         <v>166.959158</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B239" s="1">
         <v>-13.768751999999999</v>
@@ -5219,12 +5219,12 @@
         <v>-177.15609699999999</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B240" s="1">
         <v>-13.759029</v>
@@ -5233,12 +5233,12 @@
         <v>-172.10462899999999</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B241" s="1">
         <v>42.602635999999997</v>
@@ -5247,12 +5247,12 @@
         <v>20.902977</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B242" s="1">
         <v>15.552727000000001</v>
@@ -5261,12 +5261,12 @@
         <v>48.516387999999999</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="243" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B243" s="1">
         <v>-12.827500000000001</v>
@@ -5275,12 +5275,12 @@
         <v>45.166243999999999</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B244" s="1">
         <v>-30.559481999999999</v>
@@ -5289,12 +5289,12 @@
         <v>22.937505999999999</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B245" s="1">
         <v>-13.133896999999999</v>
@@ -5303,12 +5303,12 @@
         <v>27.849332</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B246" s="1">
         <v>-19.015438</v>
@@ -5317,12 +5317,12 @@
         <v>29.154857</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B247" s="1">
         <v>6.8769999999999998</v>
@@ -5331,7 +5331,7 @@
         <v>31.306999999999999</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="18" x14ac:dyDescent="0.2">

</xml_diff>